<commit_message>
Added coordinates margin to board
</commit_message>
<xml_diff>
--- a/puzzles.xlsx
+++ b/puzzles.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d25a3e113a672fd0/Documents/School/TU/Graduate/Research/Not All Explanatations Are Created Equal/chess_puzzle_explainer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="11_9081DA0BE816CA274F2C4C091D1B6EF0472C52D6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C553D3A2-E470-444A-9D73-3FBDB5E0E76A}"/>
+  <xr:revisionPtr revIDLastSave="189" documentId="11_9081DA0BE816CA274F2C4C091D1B6EF0472C52D6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0F357BF-A497-4F0C-BE7A-FFED7EB1941C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Puzzles" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
   <si>
     <t>Board</t>
   </si>
@@ -194,6 +207,69 @@
   </si>
   <si>
     <t>3k3r/1pr1b1pp/p1npB3/3RpQq1/4P3/5P2/PPP4P/1K5R w</t>
+  </si>
+  <si>
+    <t>1k1r4/pp4p1/2p4p/2PnR2P/5B2/6P1/PP3r2/1K1R4 b</t>
+  </si>
+  <si>
+    <t>d5c3 b2c3 d8d1</t>
+  </si>
+  <si>
+    <t>Discovered Attack</t>
+  </si>
+  <si>
+    <t>r5k1/ppp3pp/5p2/8/3br3/7P/1PP1B1P1/2K1R2R w</t>
+  </si>
+  <si>
+    <t>e2c4 g8f8 e1e4</t>
+  </si>
+  <si>
+    <t>r3r1k1/p4ppn/2p4p/8/3q2b1/2NBR3/PPPQ2PP/5RK1 w</t>
+  </si>
+  <si>
+    <t>d3h7 g8h7 d2d4</t>
+  </si>
+  <si>
+    <t>e5f3 g2f3 e8e1 d1e1 g4f3</t>
+  </si>
+  <si>
+    <t>r2qr1k1/pp3ppp/3p1b2/2pPn3/2P2Bb1/3P1NP1/PP3PBP/1R1QR1K1 b</t>
+  </si>
+  <si>
+    <t>5rbR/2p1p3/8/pBkPp1p1/P3P3/6PK/1P5P/8 b</t>
+  </si>
+  <si>
+    <t>g8e6 d5e6 f8h8</t>
+  </si>
+  <si>
+    <t>2kr4/1ppn1prp/nq2p3/p6Q/P7/1PN5/2PP2BP/2KR2R1 w</t>
+  </si>
+  <si>
+    <t>g2b7 b6b7 g1g7</t>
+  </si>
+  <si>
+    <t>2kb2r1/1p1b2q1/4p3/3pN3/pNpP1R1p/P1P3r1/1P2Q1PK/6R1 b</t>
+  </si>
+  <si>
+    <t>g3h3 g2h3 g7g1</t>
+  </si>
+  <si>
+    <t>8/p6Q/kp6/3pP3/PP1P4/2P3q1/3BKp2/5r2 w</t>
+  </si>
+  <si>
+    <t>b4b5 a6a5 h7a7</t>
+  </si>
+  <si>
+    <t>d1e2 f2g3 e2e3</t>
+  </si>
+  <si>
+    <t>6k1/5pp1/p1p1b2p/8/4P3/P1QpBP2/1P3KPP/3q4 b</t>
+  </si>
+  <si>
+    <t>8/8/4k3/5RP1/r4pK1/7P/6P1/8 b</t>
+  </si>
+  <si>
+    <t>f4f3 g4f3 e6f5</t>
   </si>
 </sst>
 </file>
@@ -565,17 +641,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="56.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -595,357 +671,497 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="D2">
-        <v>682</v>
+        <v>643</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3">
-        <v>802</v>
+        <v>682</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4">
-        <v>809</v>
+        <v>802</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
       </c>
       <c r="D5">
-        <v>817</v>
+        <v>809</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6">
-        <v>843</v>
+        <v>817</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D7">
-        <v>861</v>
+        <v>822</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8">
-        <v>896</v>
+        <v>843</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D9">
-        <v>1006</v>
+        <v>861</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D10">
-        <v>1039</v>
+        <v>893</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D11">
-        <v>1066</v>
+        <v>896</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D12">
-        <v>1076</v>
+        <v>914</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C13" t="s">
         <v>49</v>
       </c>
       <c r="D13">
-        <v>1079</v>
+        <v>970</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D14">
-        <v>1170</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>48</v>
       </c>
       <c r="D15">
-        <v>1210</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
         <v>48</v>
       </c>
       <c r="D16">
-        <v>1222</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D17">
-        <v>1352</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18">
-        <v>1397</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D19">
-        <v>1462</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
         <v>47</v>
       </c>
       <c r="D20">
-        <v>1503</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21">
-        <v>1522</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
         <v>48</v>
       </c>
       <c r="D22">
-        <v>1525</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D23">
-        <v>1763</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D24">
-        <v>1902</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25">
-        <v>1916</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27">
+        <v>1503</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32">
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33">
+        <v>1763</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34">
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35">
+        <v>1916</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B36" t="s">
         <v>45</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C36" t="s">
         <v>47</v>
       </c>
-      <c r="D26">
+      <c r="D36">
         <v>1997</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D26">
-    <sortCondition ref="D1:D26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D36">
+    <sortCondition ref="D1:D36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Chat can now scroll up and focus on most recent chat
</commit_message>
<xml_diff>
--- a/puzzles.xlsx
+++ b/puzzles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d25a3e113a672fd0/Documents/School/TU/Graduate/Research/Not All Explanatations Are Created Equal/chess_puzzle_explainer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="11_9081DA0BE816CA274F2C4C091D1B6EF0472C52D6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0F357BF-A497-4F0C-BE7A-FFED7EB1941C}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="11_9081DA0BE816CA274F2C4C091D1B6EF0472C52D6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0274FD91-F1F3-404A-83F6-DE0BFD8BE945}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -301,7 +301,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -316,9 +316,29 @@
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
-      </top>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -328,16 +348,76 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -352,6 +432,24 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DFED82F-92FD-491B-8BAA-05E3F37F6D1B}" name="Table1" displayName="Table1" ref="A1:D36" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="2" tableBorderDxfId="0">
+  <autoFilter ref="A1:D36" xr:uid="{8DFED82F-92FD-491B-8BAA-05E3F37F6D1B}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{A8324C6E-D011-4352-8D6A-2A658750DE6F}" name="Board"/>
+    <tableColumn id="2" xr3:uid="{41A3A1BF-3402-4AAA-8B8A-DF79498046E6}" name="Moves"/>
+    <tableColumn id="3" xr3:uid="{63C5B76C-76B3-4978-9BF6-147FDCB3AEED}" name="Theme"/>
+    <tableColumn id="4" xr3:uid="{CF9A3D85-AD2B-42C8-B903-58E20217AB35}" name="Rating"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -644,7 +742,7 @@
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection sqref="A1:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,7 +754,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -665,497 +763,497 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>643</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>682</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>802</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>809</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>817</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>822</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>843</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>861</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>893</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>896</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>914</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>970</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>1006</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>1006</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>1039</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>1066</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>1076</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>1079</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>1170</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>1210</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <v>1222</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>1273</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="4">
         <v>1352</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="A25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="4">
         <v>1397</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="4">
         <v>1462</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="4">
         <v>1503</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="A28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="4">
         <v>1522</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="4">
         <v>1525</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="A30" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="4">
         <v>1581</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="A31" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="4">
         <v>1612</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A32" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="4">
         <v>1710</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="A33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="4">
         <v>1763</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="4">
         <v>1902</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="4">
         <v>1916</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="A36" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="4">
         <v>1997</v>
       </c>
     </row>
@@ -1165,5 +1263,8 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added checks for piece to move, capture, and king checks
</commit_message>
<xml_diff>
--- a/puzzles.xlsx
+++ b/puzzles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d25a3e113a672fd0/Documents/School/TU/Graduate/Research/Not All Explanatations Are Created Equal/chess_puzzle_explainer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="195" documentId="11_9081DA0BE816CA274F2C4C091D1B6EF0472C52D6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0274FD91-F1F3-404A-83F6-DE0BFD8BE945}"/>
+  <xr:revisionPtr revIDLastSave="249" documentId="11_9081DA0BE816CA274F2C4C091D1B6EF0472C52D6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3C25FBA-BB6D-4762-82D1-3D632AE424D3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Puzzles" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
   <si>
     <t>Board</t>
   </si>
@@ -270,6 +270,27 @@
   </si>
   <si>
     <t>f4f3 g4f3 e6f5</t>
+  </si>
+  <si>
+    <t>Queen</t>
+  </si>
+  <si>
+    <t>Bishop</t>
+  </si>
+  <si>
+    <t>First Move Piece</t>
+  </si>
+  <si>
+    <t>Capture Target</t>
+  </si>
+  <si>
+    <t>King Check</t>
+  </si>
+  <si>
+    <t>Rook</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -348,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -359,7 +380,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,6 +398,13 @@
         </top>
         <bottom style="thin">
           <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
         </bottom>
       </border>
     </dxf>
@@ -410,13 +437,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -435,17 +455,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DFED82F-92FD-491B-8BAA-05E3F37F6D1B}" name="Table1" displayName="Table1" ref="A1:D36" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="2" tableBorderDxfId="0">
-  <autoFilter ref="A1:D36" xr:uid="{8DFED82F-92FD-491B-8BAA-05E3F37F6D1B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DFED82F-92FD-491B-8BAA-05E3F37F6D1B}" name="Table1" displayName="Table1" ref="A1:G36" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:G36" xr:uid="{8DFED82F-92FD-491B-8BAA-05E3F37F6D1B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="4">
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A8324C6E-D011-4352-8D6A-2A658750DE6F}" name="Board"/>
     <tableColumn id="2" xr3:uid="{41A3A1BF-3402-4AAA-8B8A-DF79498046E6}" name="Moves"/>
     <tableColumn id="3" xr3:uid="{63C5B76C-76B3-4978-9BF6-147FDCB3AEED}" name="Theme"/>
+    <tableColumn id="5" xr3:uid="{D5D6E253-3F91-4B17-B71D-D85F53F85C03}" name="First Move Piece"/>
+    <tableColumn id="6" xr3:uid="{219B08F6-24DF-4FAB-8880-6363EADBFAA6}" name="Capture Target"/>
+    <tableColumn id="7" xr3:uid="{3D2E2454-80FC-4195-9FF3-A2D0020359E6}" name="King Check"/>
     <tableColumn id="4" xr3:uid="{CF9A3D85-AD2B-42C8-B903-58E20217AB35}" name="Rating"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -739,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -750,10 +776,13 @@
     <col min="1" max="1" width="58.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -763,504 +792,525 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G2">
         <v>643</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="4">
+      <c r="G3">
         <v>682</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="4">
+      <c r="G4">
         <v>802</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="4">
+      <c r="G5">
         <v>809</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="4">
+      <c r="G6">
         <v>817</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="4">
+      <c r="G7">
         <v>822</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="4">
+      <c r="G8">
         <v>843</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="4">
+      <c r="G9">
         <v>861</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="4">
+      <c r="G10">
         <v>893</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11">
         <v>896</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="4">
+      <c r="G12">
         <v>914</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>75</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="4">
+      <c r="G13">
         <v>970</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="4">
+      <c r="G14">
         <v>1006</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="4">
+      <c r="G15">
         <v>1006</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="4">
+      <c r="G16">
         <v>1039</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="4">
+      <c r="G17">
         <v>1066</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="4">
+      <c r="G18">
         <v>1076</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="4">
+      <c r="G19">
         <v>1079</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="4">
+      <c r="G20">
         <v>1170</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="4">
+      <c r="G21">
         <v>1210</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="4">
+      <c r="G22">
         <v>1222</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="D23" s="4">
+      <c r="G23">
         <v>1273</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="4">
+      <c r="G24">
         <v>1352</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="4">
+      <c r="G25">
         <v>1397</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="4">
+      <c r="G26">
         <v>1462</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="4">
+      <c r="G27">
         <v>1503</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="4">
+      <c r="G28">
         <v>1522</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="4">
+      <c r="G29">
         <v>1525</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" t="s">
         <v>72</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="4">
+      <c r="G30">
         <v>1581</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>66</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="4">
+      <c r="G31">
         <v>1612</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="4">
+      <c r="G32">
         <v>1710</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="C33" t="s">
         <v>47</v>
       </c>
-      <c r="D33" s="4">
+      <c r="G33">
         <v>1763</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="4">
+      <c r="G34">
         <v>1902</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="4">
+      <c r="G35">
         <v>1916</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="4">
+      <c r="G36">
         <v>1997</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D36">
-    <sortCondition ref="D1:D36"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Corrected puzzles excel file
</commit_message>
<xml_diff>
--- a/puzzles.xlsx
+++ b/puzzles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d25a3e113a672fd0/Documents/School/TU/Graduate/Research/Not All Explanatations Are Created Equal/chess_puzzle_explainer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="249" documentId="11_9081DA0BE816CA274F2C4C091D1B6EF0472C52D6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3C25FBA-BB6D-4762-82D1-3D632AE424D3}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="11_9081DA0BE816CA274F2C4C091D1B6EF0472C52D6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93E5749B-1937-4150-98B9-67CD7ADA799B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Puzzles" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
   <si>
     <t>Board</t>
   </si>
@@ -270,27 +270,6 @@
   </si>
   <si>
     <t>f4f3 g4f3 e6f5</t>
-  </si>
-  <si>
-    <t>Queen</t>
-  </si>
-  <si>
-    <t>Bishop</t>
-  </si>
-  <si>
-    <t>First Move Piece</t>
-  </si>
-  <si>
-    <t>Capture Target</t>
-  </si>
-  <si>
-    <t>King Check</t>
-  </si>
-  <si>
-    <t>Rook</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -455,23 +434,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DFED82F-92FD-491B-8BAA-05E3F37F6D1B}" name="Table1" displayName="Table1" ref="A1:G36" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:G36" xr:uid="{8DFED82F-92FD-491B-8BAA-05E3F37F6D1B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8DFED82F-92FD-491B-8BAA-05E3F37F6D1B}" name="Table1" displayName="Table1" ref="A1:D36" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:D36" xr:uid="{8DFED82F-92FD-491B-8BAA-05E3F37F6D1B}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
   </autoFilter>
-  <tableColumns count="7">
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A8324C6E-D011-4352-8D6A-2A658750DE6F}" name="Board"/>
     <tableColumn id="2" xr3:uid="{41A3A1BF-3402-4AAA-8B8A-DF79498046E6}" name="Moves"/>
     <tableColumn id="3" xr3:uid="{63C5B76C-76B3-4978-9BF6-147FDCB3AEED}" name="Theme"/>
-    <tableColumn id="5" xr3:uid="{D5D6E253-3F91-4B17-B71D-D85F53F85C03}" name="First Move Piece"/>
-    <tableColumn id="6" xr3:uid="{219B08F6-24DF-4FAB-8880-6363EADBFAA6}" name="Capture Target"/>
-    <tableColumn id="7" xr3:uid="{3D2E2454-80FC-4195-9FF3-A2D0020359E6}" name="King Check"/>
     <tableColumn id="4" xr3:uid="{CF9A3D85-AD2B-42C8-B903-58E20217AB35}" name="Rating"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -765,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,13 +749,10 @@
     <col min="1" max="1" width="58.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -792,20 +762,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>61</v>
       </c>
@@ -815,20 +776,11 @@
       <c r="C2" t="s">
         <v>60</v>
       </c>
-      <c r="D2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G2">
+      <c r="D2">
         <v>643</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -838,11 +790,11 @@
       <c r="C3" t="s">
         <v>46</v>
       </c>
-      <c r="G3">
+      <c r="D3">
         <v>682</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -852,11 +804,11 @@
       <c r="C4" t="s">
         <v>47</v>
       </c>
-      <c r="G4">
+      <c r="D4">
         <v>802</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -866,11 +818,11 @@
       <c r="C5" t="s">
         <v>46</v>
       </c>
-      <c r="G5">
+      <c r="D5">
         <v>809</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -880,11 +832,11 @@
       <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="G6">
+      <c r="D6">
         <v>817</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>63</v>
       </c>
@@ -894,11 +846,11 @@
       <c r="C7" t="s">
         <v>60</v>
       </c>
-      <c r="G7">
+      <c r="D7">
         <v>822</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -908,11 +860,11 @@
       <c r="C8" t="s">
         <v>47</v>
       </c>
-      <c r="G8">
+      <c r="D8">
         <v>843</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -922,11 +874,11 @@
       <c r="C9" t="s">
         <v>49</v>
       </c>
-      <c r="G9">
+      <c r="D9">
         <v>861</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -936,11 +888,11 @@
       <c r="C10" t="s">
         <v>60</v>
       </c>
-      <c r="G10">
+      <c r="D10">
         <v>893</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -950,17 +902,11 @@
       <c r="C11" t="s">
         <v>48</v>
       </c>
-      <c r="D11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11">
+      <c r="D11">
         <v>896</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -970,11 +916,11 @@
       <c r="C12" t="s">
         <v>49</v>
       </c>
-      <c r="G12">
+      <c r="D12">
         <v>914</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>76</v>
       </c>
@@ -984,11 +930,11 @@
       <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="G13">
+      <c r="D13">
         <v>970</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -998,11 +944,11 @@
       <c r="C14" t="s">
         <v>60</v>
       </c>
-      <c r="G14">
+      <c r="D14">
         <v>1006</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1012,11 +958,11 @@
       <c r="C15" t="s">
         <v>48</v>
       </c>
-      <c r="G15">
+      <c r="D15">
         <v>1006</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -1026,11 +972,11 @@
       <c r="C16" t="s">
         <v>48</v>
       </c>
-      <c r="G16">
+      <c r="D16">
         <v>1039</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1040,11 +986,11 @@
       <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="G17">
+      <c r="D17">
         <v>1066</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1054,11 +1000,11 @@
       <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="G18">
+      <c r="D18">
         <v>1076</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -1068,11 +1014,11 @@
       <c r="C19" t="s">
         <v>49</v>
       </c>
-      <c r="G19">
+      <c r="D19">
         <v>1079</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -1082,11 +1028,11 @@
       <c r="C20" t="s">
         <v>47</v>
       </c>
-      <c r="G20">
+      <c r="D20">
         <v>1170</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -1096,11 +1042,11 @@
       <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="G21">
+      <c r="D21">
         <v>1210</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -1110,11 +1056,11 @@
       <c r="C22" t="s">
         <v>48</v>
       </c>
-      <c r="G22">
+      <c r="D22">
         <v>1222</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -1124,11 +1070,11 @@
       <c r="C23" t="s">
         <v>60</v>
       </c>
-      <c r="G23">
+      <c r="D23">
         <v>1273</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1138,11 +1084,11 @@
       <c r="C24" t="s">
         <v>49</v>
       </c>
-      <c r="G24">
+      <c r="D24">
         <v>1352</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -1152,11 +1098,11 @@
       <c r="C25" t="s">
         <v>47</v>
       </c>
-      <c r="G25">
+      <c r="D25">
         <v>1397</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -1166,11 +1112,11 @@
       <c r="C26" t="s">
         <v>46</v>
       </c>
-      <c r="G26">
+      <c r="D26">
         <v>1462</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -1180,11 +1126,11 @@
       <c r="C27" t="s">
         <v>47</v>
       </c>
-      <c r="G27">
+      <c r="D27">
         <v>1503</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -1194,11 +1140,11 @@
       <c r="C28" t="s">
         <v>49</v>
       </c>
-      <c r="G28">
+      <c r="D28">
         <v>1522</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>20</v>
       </c>
@@ -1208,11 +1154,11 @@
       <c r="C29" t="s">
         <v>48</v>
       </c>
-      <c r="G29">
+      <c r="D29">
         <v>1525</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -1222,11 +1168,11 @@
       <c r="C30" t="s">
         <v>60</v>
       </c>
-      <c r="G30">
+      <c r="D30">
         <v>1581</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>66</v>
       </c>
@@ -1236,11 +1182,11 @@
       <c r="C31" t="s">
         <v>60</v>
       </c>
-      <c r="G31">
+      <c r="D31">
         <v>1612</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -1250,11 +1196,11 @@
       <c r="C32" t="s">
         <v>49</v>
       </c>
-      <c r="G32">
+      <c r="D32">
         <v>1710</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>21</v>
       </c>
@@ -1264,11 +1210,11 @@
       <c r="C33" t="s">
         <v>47</v>
       </c>
-      <c r="G33">
+      <c r="D33">
         <v>1763</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -1278,11 +1224,11 @@
       <c r="C34" t="s">
         <v>46</v>
       </c>
-      <c r="G34">
+      <c r="D34">
         <v>1902</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1292,11 +1238,11 @@
       <c r="C35" t="s">
         <v>48</v>
       </c>
-      <c r="G35">
+      <c r="D35">
         <v>1916</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1306,7 +1252,7 @@
       <c r="C36" t="s">
         <v>47</v>
       </c>
-      <c r="G36">
+      <c r="D36">
         <v>1997</v>
       </c>
     </row>

</xml_diff>